<commit_message>
Tracks first and second game, updates scraper to handle multiple-spaced last names and baserunning events, updates pitch tracker to auto-fill strikeouts and prompt for balls in play
</commit_message>
<xml_diff>
--- a/data-dictionary.xlsx
+++ b/data-dictionary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackhinde/baycats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED11DF2-1AAF-5544-B660-8B4C357C7E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEE27A1-ABD6-CB4D-8643-8A09D284831F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{DFFC6746-A55A-9546-8420-2CE97E2823F2}"/>
+    <workbookView xWindow="48300" yWindow="-2560" windowWidth="14280" windowHeight="16280" xr2:uid="{DFFC6746-A55A-9546-8420-2CE97E2823F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -140,9 +140,6 @@
     <t>Short hand of pitch result. B = ball, S = strike, X = in play.</t>
   </si>
   <si>
-    <t>B, S, X</t>
-  </si>
-  <si>
     <t>hit_location</t>
   </si>
   <si>
@@ -359,9 +356,6 @@
     <t>The name of the pitch derived from the Statcast Data.</t>
   </si>
   <si>
-    <t>4-Seam Fastball, Changeup, Curveball, Cutter, Eephus, Forkball, Knuckle Curve, Knuckleball, Other, Pitch Out, Screwball, Sinker, Slider, Slow Curve, Slurve, Split-Finger, Sweeper</t>
-  </si>
-  <si>
     <t>home_score</t>
   </si>
   <si>
@@ -507,6 +501,12 @@
   </si>
   <si>
     <t>Undecided whether or not to track, NOT currently tracked</t>
+  </si>
+  <si>
+    <t>Four-Seam Fastball, Changeup, Curveball, Cutter, Eephus, Forkball, Knuckle Curve, Knuckleball, Other, Pitch Out, Screwball, Sinker, Slider, Slow Curve, Slurve, Split-Finger, Sweeper</t>
+  </si>
+  <si>
+    <t>B, E, S, U, X</t>
   </si>
 </sst>
 </file>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46951226-35B7-A64E-A4E8-5ECED1EA1B08}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,7 +996,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1013,10 +1013,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>5</v>
@@ -1052,21 +1052,21 @@
         <v>22</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>19</v>
@@ -1075,10 +1075,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1148,7 +1148,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1188,15 +1188,15 @@
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>19</v>
@@ -1205,24 +1205,24 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>19</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>19</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
@@ -1255,10 +1255,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>19</v>
@@ -1267,16 +1267,16 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1295,10 +1295,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>9</v>
@@ -1307,10 +1307,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>9</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>9</v>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>9</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>9</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="31" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>97</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>98</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>19</v>
@@ -1379,24 +1379,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="C32" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>5</v>
@@ -1405,10 +1405,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>5</v>
@@ -1417,10 +1417,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>5</v>
@@ -1429,10 +1429,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>5</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>5</v>
@@ -1453,10 +1453,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>5</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>5</v>
@@ -1477,10 +1477,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>5</v>
@@ -1489,10 +1489,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>5</v>
@@ -1501,10 +1501,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>5</v>
@@ -1513,10 +1513,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>5</v>
@@ -1525,10 +1525,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>19</v>
@@ -1537,10 +1537,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>19</v>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>19</v>
@@ -1561,10 +1561,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>19</v>
@@ -1573,10 +1573,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>19</v>
@@ -1585,10 +1585,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>19</v>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>19</v>
@@ -1609,10 +1609,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>19</v>
@@ -1621,10 +1621,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>19</v>
@@ -1633,10 +1633,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>19</v>
@@ -1645,10 +1645,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>9</v>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>9</v>
@@ -1669,10 +1669,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>9</v>
@@ -1681,10 +1681,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>9</v>
@@ -1693,24 +1693,24 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>19</v>
@@ -1719,10 +1719,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>19</v>
@@ -1731,10 +1731,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>19</v>
@@ -1743,10 +1743,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>19</v>
@@ -1755,10 +1755,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>19</v>
@@ -1767,83 +1767,83 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="11"/>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="14"/>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds batted ball and plate discipline tables to batter helper. Edits scraper to handle substitutions of players with non FirstName LastName names.
</commit_message>
<xml_diff>
--- a/data-dictionary.xlsx
+++ b/data-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackhinde/baycats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CAD5CA-FEA1-FB44-9B39-0375E041D850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72F1A84-E094-224A-91E4-47B14E9F1390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="5120" windowWidth="14280" windowHeight="16280" xr2:uid="{DFFC6746-A55A-9546-8420-2CE97E2823F2}"/>
+    <workbookView xWindow="29860" yWindow="-2680" windowWidth="17860" windowHeight="16280" xr2:uid="{DFFC6746-A55A-9546-8420-2CE97E2823F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>Batted ball type, ground_ball, line_drive, fly_ball, popup.</t>
   </si>
   <si>
-    <t>fly_ball, ground_ball, line_drive, popup</t>
-  </si>
-  <si>
     <t>balls</t>
   </si>
   <si>
@@ -507,6 +504,9 @@
   </si>
   <si>
     <t>B, E, S, U, X</t>
+  </si>
+  <si>
+    <t>bunt, fly_ball, ground_ball, line_drive, popup</t>
   </si>
 </sst>
 </file>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46951226-35B7-A64E-A4E8-5ECED1EA1B08}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,7 +996,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1013,10 +1013,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>5</v>
@@ -1052,21 +1052,21 @@
         <v>22</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>19</v>
@@ -1075,10 +1075,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1148,7 +1148,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1214,15 +1214,15 @@
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>19</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>19</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
@@ -1255,10 +1255,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>19</v>
@@ -1267,16 +1267,16 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1295,10 +1295,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>9</v>
@@ -1307,10 +1307,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>9</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>9</v>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>9</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>9</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="31" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>19</v>
@@ -1379,24 +1379,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>103</v>
-      </c>
       <c r="C32" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>5</v>
@@ -1405,10 +1405,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>5</v>
@@ -1417,10 +1417,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>5</v>
@@ -1429,10 +1429,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>5</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>5</v>
@@ -1453,10 +1453,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>5</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>5</v>
@@ -1477,10 +1477,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>5</v>
@@ -1489,10 +1489,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>5</v>
@@ -1501,10 +1501,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>5</v>
@@ -1513,10 +1513,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>5</v>
@@ -1525,10 +1525,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>19</v>
@@ -1537,10 +1537,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>19</v>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>19</v>
@@ -1561,10 +1561,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>19</v>
@@ -1573,10 +1573,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>19</v>
@@ -1585,10 +1585,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>19</v>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>19</v>
@@ -1609,10 +1609,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>19</v>
@@ -1621,10 +1621,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>19</v>
@@ -1633,10 +1633,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>19</v>
@@ -1645,10 +1645,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>9</v>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>9</v>
@@ -1669,10 +1669,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>9</v>
@@ -1681,10 +1681,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>9</v>
@@ -1693,24 +1693,24 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>130</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>19</v>
@@ -1719,10 +1719,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" s="14" t="s">
         <v>131</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>132</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>19</v>
@@ -1731,10 +1731,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>19</v>
@@ -1743,10 +1743,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>19</v>
@@ -1755,10 +1755,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>19</v>
@@ -1767,83 +1767,83 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="C64" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="C65" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="11"/>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
       <c r="B69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="14"/>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>